<commit_message>
Diseño acabado a falta de mostrar los corredores
</commit_message>
<xml_diff>
--- a/StartListMaker/equipos.xlsx
+++ b/StartListMaker/equipos.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Solvay Cycling Team</t>
   </si>
   <si>
-    <t xml:space="preserve">Team Tine – Danfoss</t>
+    <t xml:space="preserve">Team Tine - Danfoss</t>
   </si>
   <si>
     <t xml:space="preserve">Milka</t>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">Eritrean Airlines</t>
   </si>
   <si>
-    <t xml:space="preserve">Konami – Yokohama</t>
+    <t xml:space="preserve">Konami - Yokohama</t>
   </si>
   <si>
     <t xml:space="preserve">Harley Davidson</t>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">Pralines Leonidas</t>
   </si>
   <si>
-    <t xml:space="preserve">Fanox – Bizkaia</t>
+    <t xml:space="preserve">Fanox - Bizkaia</t>
   </si>
   <si>
     <t xml:space="preserve">Lapierre Pro Team</t>
@@ -82,16 +82,25 @@
     <t xml:space="preserve">Lenta</t>
   </si>
   <si>
+    <t xml:space="preserve">Ciudad de Medellin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saxo Bank - Sungard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manuela Fundacion</t>
+  </si>
+  <si>
     <t xml:space="preserve">Adriatic.hr</t>
   </si>
   <si>
-    <t xml:space="preserve">Barclays – Engie</t>
+    <t xml:space="preserve">Barclays - Engie</t>
   </si>
   <si>
     <t xml:space="preserve">Nutella Pro Team</t>
   </si>
   <si>
-    <t xml:space="preserve">Boels – Dolmans</t>
+    <t xml:space="preserve">Boels - Dolmans</t>
   </si>
   <si>
     <t xml:space="preserve">Acqua &amp; Sapone</t>
@@ -100,28 +109,19 @@
     <t xml:space="preserve">Omega Pharma</t>
   </si>
   <si>
-    <t xml:space="preserve">Frigo – Philips</t>
+    <t xml:space="preserve">Frigo - Philips</t>
   </si>
   <si>
     <t xml:space="preserve">OTIS Cycling Team</t>
   </si>
   <si>
+    <t xml:space="preserve">Saunier Duval</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tissot</t>
   </si>
   <si>
     <t xml:space="preserve">Televisión</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ciudad de Medellin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saxo Bank – Sungard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manuela Fundacion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saunier Duval</t>
   </si>
 </sst>
 </file>
@@ -239,7 +239,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -395,7 +395,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>19</v>
@@ -403,7 +403,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>20</v>
@@ -411,7 +411,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>21</v>
@@ -419,7 +419,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>22</v>
@@ -427,7 +427,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>23</v>
@@ -435,7 +435,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>24</v>
@@ -443,7 +443,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>25</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>26</v>
@@ -459,7 +459,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>27</v>
@@ -467,7 +467,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>28</v>
@@ -475,7 +475,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>29</v>
@@ -483,7 +483,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>30</v>
@@ -491,7 +491,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>31</v>
@@ -499,7 +499,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>32</v>

</xml_diff>